<commit_message>
Include population data for 2023.
</commit_message>
<xml_diff>
--- a/data-raw/files/population/Personer_svalbard_1990-2020.xlsx
+++ b/data-raw/files/population/Personer_svalbard_1990-2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/home/git/fhidata/inst/rawdata/population/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/containers/volumes/workbench/r-packages/csdata/data-raw/files/population/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D90D801-1744-7548-B1B7-A0B5D78F0BD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4343466-7970-1F4A-A15D-F461C26CEE2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="500" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4420" yWindow="19860" windowWidth="38620" windowHeight="8820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Personer" sheetId="2" r:id="rId1"/>
@@ -105,12 +105,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,554 +412,568 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI5"/>
+  <dimension ref="A1:AJ5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="AI2" sqref="AI2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="AJ2" sqref="AJ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11" style="1" customWidth="1"/>
-    <col min="4" max="32" width="9.33203125" style="1" customWidth="1"/>
-    <col min="33" max="35" width="9.33203125" style="3" customWidth="1"/>
-    <col min="36" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="40.6640625" customWidth="1"/>
+    <col min="2" max="2" width="8.5" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="32" width="9.33203125" customWidth="1"/>
+    <col min="33" max="35" width="9.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1">
+      <c r="B1">
         <v>1990</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C1">
         <v>1991</v>
       </c>
-      <c r="D1" s="1">
+      <c r="D1">
         <v>1992</v>
       </c>
-      <c r="E1" s="1">
+      <c r="E1">
         <v>1993</v>
       </c>
-      <c r="F1" s="1">
+      <c r="F1">
         <v>1994</v>
       </c>
-      <c r="G1" s="1">
+      <c r="G1">
         <v>1995</v>
       </c>
-      <c r="H1" s="1">
+      <c r="H1">
         <v>1996</v>
       </c>
-      <c r="I1" s="1">
+      <c r="I1">
         <v>1997</v>
       </c>
-      <c r="J1" s="1">
+      <c r="J1">
         <v>1998</v>
       </c>
-      <c r="K1" s="1">
+      <c r="K1">
         <v>1999</v>
       </c>
-      <c r="L1" s="1">
+      <c r="L1">
         <v>2000</v>
       </c>
-      <c r="M1" s="1">
+      <c r="M1">
         <v>2001</v>
       </c>
-      <c r="N1" s="1">
+      <c r="N1">
         <v>2002</v>
       </c>
-      <c r="O1" s="1">
+      <c r="O1">
         <v>2003</v>
       </c>
-      <c r="P1" s="1">
+      <c r="P1">
         <v>2004</v>
       </c>
-      <c r="Q1" s="1">
+      <c r="Q1">
         <v>2005</v>
       </c>
-      <c r="R1" s="1">
+      <c r="R1">
         <v>2006</v>
       </c>
-      <c r="S1" s="1">
+      <c r="S1">
         <v>2007</v>
       </c>
-      <c r="T1" s="1">
+      <c r="T1">
         <v>2008</v>
       </c>
-      <c r="U1" s="1">
+      <c r="U1">
         <v>2009</v>
       </c>
-      <c r="V1" s="1">
+      <c r="V1">
         <v>2010</v>
       </c>
-      <c r="W1" s="1">
+      <c r="W1">
         <v>2011</v>
       </c>
-      <c r="X1" s="1">
+      <c r="X1">
         <v>2012</v>
       </c>
-      <c r="Y1" s="1">
+      <c r="Y1">
         <v>2013</v>
       </c>
-      <c r="Z1" s="1">
+      <c r="Z1">
         <v>2014</v>
       </c>
-      <c r="AA1" s="1">
+      <c r="AA1">
         <v>2015</v>
       </c>
-      <c r="AB1" s="1">
+      <c r="AB1">
         <v>2016</v>
       </c>
-      <c r="AC1" s="1">
+      <c r="AC1">
         <v>2017</v>
       </c>
-      <c r="AD1" s="1">
+      <c r="AD1">
         <v>2018</v>
       </c>
-      <c r="AE1" s="1">
+      <c r="AE1">
         <v>2019</v>
       </c>
-      <c r="AF1" s="1">
+      <c r="AF1">
         <v>2020</v>
       </c>
-      <c r="AG1" s="3">
+      <c r="AG1" s="2">
         <v>2021</v>
       </c>
-      <c r="AH1" s="3">
+      <c r="AH1" s="2">
         <v>2022</v>
       </c>
-      <c r="AI1" s="3">
+      <c r="AI1" s="2">
         <v>2023</v>
       </c>
+      <c r="AJ1" s="2">
+        <v>2024</v>
+      </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
         <v>1125</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>1135</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>1148</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>1050</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="1">
         <v>1097</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="1">
         <v>1218</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="1">
         <v>1230</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="1">
         <v>1335</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="1">
         <v>1438</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="1">
         <v>1476</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2" s="1">
         <v>1475</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2" s="1">
         <v>1704</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2" s="1">
         <v>1570</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O2" s="1">
         <v>1562</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P2" s="1">
         <v>1581</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="Q2" s="1">
         <v>1645</v>
       </c>
-      <c r="R2" s="2">
+      <c r="R2" s="1">
         <v>1721</v>
       </c>
-      <c r="S2" s="2">
+      <c r="S2" s="1">
         <v>1781</v>
       </c>
-      <c r="T2" s="2">
+      <c r="T2" s="1">
         <v>1821</v>
       </c>
-      <c r="U2" s="2">
+      <c r="U2" s="1">
         <v>1792</v>
       </c>
-      <c r="V2" s="2">
+      <c r="V2" s="1">
         <v>1744</v>
       </c>
-      <c r="W2" s="2">
+      <c r="W2" s="1">
         <v>1695</v>
       </c>
-      <c r="X2" s="2">
+      <c r="X2" s="1">
         <v>1738</v>
       </c>
-      <c r="Y2" s="2">
+      <c r="Y2" s="1">
         <v>1748</v>
       </c>
-      <c r="Z2" s="2">
+      <c r="Z2" s="1">
         <v>1662</v>
       </c>
-      <c r="AA2" s="2">
+      <c r="AA2" s="1">
         <v>1692</v>
       </c>
-      <c r="AB2" s="2">
+      <c r="AB2" s="1">
         <v>1614</v>
       </c>
-      <c r="AC2" s="2">
+      <c r="AC2" s="1">
         <v>1565</v>
       </c>
-      <c r="AD2" s="2">
+      <c r="AD2" s="1">
         <v>1555</v>
       </c>
-      <c r="AE2" s="2">
+      <c r="AE2" s="1">
         <v>1581</v>
       </c>
-      <c r="AF2" s="2">
+      <c r="AF2" s="1">
         <v>1697</v>
       </c>
-      <c r="AG2" s="4">
-        <v>1697</v>
-      </c>
-      <c r="AH2" s="4">
-        <v>1697</v>
-      </c>
-      <c r="AI2" s="4">
-        <v>1697</v>
+      <c r="AG2" s="3">
+        <v>1706</v>
+      </c>
+      <c r="AH2" s="3">
+        <v>1753</v>
+      </c>
+      <c r="AI2" s="3">
+        <v>1753</v>
+      </c>
+      <c r="AJ2" s="3">
+        <v>1753</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2">
-        <v>0</v>
-      </c>
-      <c r="I3" s="2">
-        <v>0</v>
-      </c>
-      <c r="J3" s="2">
-        <v>0</v>
-      </c>
-      <c r="K3" s="2">
-        <v>0</v>
-      </c>
-      <c r="L3" s="2">
-        <v>0</v>
-      </c>
-      <c r="M3" s="2">
-        <v>0</v>
-      </c>
-      <c r="N3" s="2">
-        <v>0</v>
-      </c>
-      <c r="O3" s="2">
-        <v>0</v>
-      </c>
-      <c r="P3" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="2">
-        <v>0</v>
-      </c>
-      <c r="R3" s="2">
-        <v>0</v>
-      </c>
-      <c r="S3" s="2">
-        <v>0</v>
-      </c>
-      <c r="T3" s="2">
-        <v>0</v>
-      </c>
-      <c r="U3" s="2">
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0</v>
+      </c>
+      <c r="P3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>0</v>
+      </c>
+      <c r="R3" s="1">
+        <v>0</v>
+      </c>
+      <c r="S3" s="1">
+        <v>0</v>
+      </c>
+      <c r="T3" s="1">
+        <v>0</v>
+      </c>
+      <c r="U3" s="1">
         <v>293</v>
       </c>
-      <c r="V3" s="2">
+      <c r="V3" s="1">
         <v>308</v>
       </c>
-      <c r="W3" s="2">
+      <c r="W3" s="1">
         <v>322</v>
       </c>
-      <c r="X3" s="2">
+      <c r="X3" s="1">
         <v>377</v>
       </c>
-      <c r="Y3" s="2">
+      <c r="Y3" s="1">
         <v>410</v>
       </c>
-      <c r="Z3" s="2">
+      <c r="Z3" s="1">
         <v>438</v>
       </c>
-      <c r="AA3" s="2">
+      <c r="AA3" s="1">
         <v>493</v>
       </c>
-      <c r="AB3" s="2">
+      <c r="AB3" s="1">
         <v>538</v>
       </c>
-      <c r="AC3" s="2">
+      <c r="AC3" s="1">
         <v>580</v>
       </c>
-      <c r="AD3" s="2">
+      <c r="AD3" s="1">
         <v>659</v>
       </c>
-      <c r="AE3" s="2">
+      <c r="AE3" s="1">
         <v>677</v>
       </c>
-      <c r="AF3" s="2">
+      <c r="AF3" s="1">
         <v>731</v>
       </c>
-      <c r="AG3" s="4">
-        <v>731</v>
-      </c>
-      <c r="AH3" s="4">
-        <v>731</v>
-      </c>
-      <c r="AI3" s="4">
-        <v>731</v>
+      <c r="AG3" s="3">
+        <v>753</v>
+      </c>
+      <c r="AH3" s="3">
+        <v>751</v>
+      </c>
+      <c r="AI3" s="3">
+        <v>751</v>
+      </c>
+      <c r="AJ3" s="3">
+        <v>751</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>2407</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>2260</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>2151</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>1958</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>1870</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <v>1679</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="1">
         <v>1604</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="1">
         <v>1482</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="1">
         <v>1149</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="1">
         <v>939</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4" s="1">
         <v>893</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4" s="1">
         <v>903</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="1">
         <v>950</v>
       </c>
-      <c r="O4" s="2">
+      <c r="O4" s="1">
         <v>918</v>
       </c>
-      <c r="P4" s="2">
+      <c r="P4" s="1">
         <v>786</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="Q4" s="1">
         <v>747</v>
       </c>
-      <c r="R4" s="2">
+      <c r="R4" s="1">
         <v>535</v>
       </c>
-      <c r="S4" s="2">
+      <c r="S4" s="1">
         <v>550</v>
       </c>
-      <c r="T4" s="2">
+      <c r="T4" s="1">
         <v>620</v>
       </c>
-      <c r="U4" s="2">
+      <c r="U4" s="1">
         <v>470</v>
       </c>
-      <c r="V4" s="2">
+      <c r="V4" s="1">
         <v>420</v>
       </c>
-      <c r="W4" s="2">
+      <c r="W4" s="1">
         <v>370</v>
       </c>
-      <c r="X4" s="2">
+      <c r="X4" s="1">
         <v>380</v>
       </c>
-      <c r="Y4" s="2">
+      <c r="Y4" s="1">
         <v>471</v>
       </c>
-      <c r="Z4" s="2">
+      <c r="Z4" s="1">
         <v>436</v>
       </c>
-      <c r="AA4" s="2">
+      <c r="AA4" s="1">
         <v>471</v>
       </c>
-      <c r="AB4" s="2">
+      <c r="AB4" s="1">
         <v>492</v>
       </c>
-      <c r="AC4" s="2">
+      <c r="AC4" s="1">
         <v>428</v>
       </c>
-      <c r="AD4" s="2">
+      <c r="AD4" s="1">
         <v>514</v>
       </c>
-      <c r="AE4" s="2">
+      <c r="AE4" s="1">
         <v>458</v>
       </c>
-      <c r="AF4" s="2">
+      <c r="AF4" s="1">
         <v>501</v>
       </c>
-      <c r="AG4" s="4">
-        <v>501</v>
-      </c>
-      <c r="AH4" s="4">
-        <v>501</v>
-      </c>
-      <c r="AI4" s="4">
-        <v>501</v>
+      <c r="AG4" s="3">
+        <v>400</v>
+      </c>
+      <c r="AH4" s="3">
+        <v>391</v>
+      </c>
+      <c r="AI4" s="3">
+        <v>391</v>
+      </c>
+      <c r="AJ4" s="3">
+        <v>391</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>12</v>
       </c>
-      <c r="C5" s="2">
-        <v>10</v>
-      </c>
-      <c r="D5" s="2">
-        <v>10</v>
-      </c>
-      <c r="E5" s="2">
+      <c r="C5" s="1">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1">
         <v>9</v>
       </c>
-      <c r="F5" s="2">
-        <v>10</v>
-      </c>
-      <c r="G5" s="2">
+      <c r="F5" s="1">
+        <v>10</v>
+      </c>
+      <c r="G5" s="1">
         <v>9</v>
       </c>
-      <c r="H5" s="2">
-        <v>10</v>
-      </c>
-      <c r="I5" s="2">
-        <v>10</v>
-      </c>
-      <c r="J5" s="2">
+      <c r="H5" s="1">
+        <v>10</v>
+      </c>
+      <c r="I5" s="1">
+        <v>10</v>
+      </c>
+      <c r="J5" s="1">
         <v>9</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="1">
         <v>8</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="1">
         <v>8</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="1">
         <v>9</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5" s="1">
         <v>9</v>
       </c>
-      <c r="O5" s="2">
+      <c r="O5" s="1">
         <v>9</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5" s="1">
         <v>8</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="Q5" s="1">
         <v>8</v>
       </c>
-      <c r="R5" s="2">
-        <v>10</v>
-      </c>
-      <c r="S5" s="2">
+      <c r="R5" s="1">
+        <v>10</v>
+      </c>
+      <c r="S5" s="1">
         <v>7</v>
       </c>
-      <c r="T5" s="2">
+      <c r="T5" s="1">
         <v>8</v>
       </c>
-      <c r="U5" s="2">
-        <v>10</v>
-      </c>
-      <c r="V5" s="2">
+      <c r="U5" s="1">
+        <v>10</v>
+      </c>
+      <c r="V5" s="1">
         <v>9</v>
       </c>
-      <c r="W5" s="2">
+      <c r="W5" s="1">
         <v>7</v>
       </c>
-      <c r="X5" s="2">
+      <c r="X5" s="1">
         <v>9</v>
       </c>
-      <c r="Y5" s="2">
+      <c r="Y5" s="1">
         <v>8</v>
       </c>
-      <c r="Z5" s="2">
-        <v>10</v>
-      </c>
-      <c r="AA5" s="2">
-        <v>10</v>
-      </c>
-      <c r="AB5" s="2">
-        <v>10</v>
-      </c>
-      <c r="AC5" s="2">
-        <v>10</v>
-      </c>
-      <c r="AD5" s="2">
-        <v>10</v>
-      </c>
-      <c r="AE5" s="2">
-        <v>10</v>
-      </c>
-      <c r="AF5" s="2">
-        <v>10</v>
-      </c>
-      <c r="AG5" s="4">
-        <v>10</v>
-      </c>
-      <c r="AH5" s="4">
-        <v>10</v>
-      </c>
-      <c r="AI5" s="4">
+      <c r="Z5" s="1">
+        <v>10</v>
+      </c>
+      <c r="AA5" s="1">
+        <v>10</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>10</v>
+      </c>
+      <c r="AC5" s="1">
+        <v>10</v>
+      </c>
+      <c r="AD5" s="1">
+        <v>10</v>
+      </c>
+      <c r="AE5" s="1">
+        <v>10</v>
+      </c>
+      <c r="AF5" s="1">
+        <v>10</v>
+      </c>
+      <c r="AG5" s="3">
+        <v>10</v>
+      </c>
+      <c r="AH5" s="3">
+        <v>10</v>
+      </c>
+      <c r="AI5" s="3">
+        <v>10</v>
+      </c>
+      <c r="AJ5" s="3">
         <v>10</v>
       </c>
     </row>

</xml_diff>